<commit_message>
Update Fixed and Donate added
- Update of db fixed
- Upload photo feature added in profile
- Logo added to all pages
- Donation add, update and remove features added
</commit_message>
<xml_diff>
--- a/static/files/business.xlsx
+++ b/static/files/business.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
   <si>
     <t>Id</t>
   </si>
@@ -58,42 +58,51 @@
     <t>Location</t>
   </si>
   <si>
-    <t>tyu</t>
+    <t>xc</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>cx</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>xcx</t>
+  </si>
+  <si>
+    <t>cxc</t>
+  </si>
+  <si>
+    <t>cxcx</t>
+  </si>
+  <si>
+    <t>lkj</t>
+  </si>
+  <si>
+    <t>lkjl</t>
+  </si>
+  <si>
+    <t>kjl</t>
+  </si>
+  <si>
+    <t>klk</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>lk</t>
+  </si>
+  <si>
+    <t>Lakshadweep</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>ty</t>
-  </si>
-  <si>
-    <t>Tamil Nadu</t>
-  </si>
-  <si>
-    <t>tyyu</t>
-  </si>
-  <si>
-    <t>lkj</t>
-  </si>
-  <si>
-    <t>lkjl</t>
-  </si>
-  <si>
-    <t>kjl</t>
-  </si>
-  <si>
-    <t>klk</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>lk</t>
-  </si>
-  <si>
-    <t>Lakshadweep</t>
-  </si>
-  <si>
     <t>hjk</t>
   </si>
   <si>
@@ -103,7 +112,13 @@
     <t>ghj</t>
   </si>
   <si>
-    <t>kkkkkk</t>
+    <t>kkkkkkokokok</t>
+  </si>
+  <si>
+    <t>sdfghjkl</t>
+  </si>
+  <si>
+    <t>asdfghjklqwertyuiopzxcvbnm</t>
   </si>
   <si>
     <t>kjkl</t>
@@ -112,19 +127,10 @@
     <t>jl</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>jklj</t>
-  </si>
-  <si>
-    <t>jkj</t>
-  </si>
-  <si>
-    <t>kj</t>
-  </si>
-  <si>
-    <t>Karnataka</t>
+    <t>okokok</t>
+  </si>
+  <si>
+    <t>Dadra and Nagar Haveli</t>
   </si>
 </sst>
 </file>
@@ -536,31 +542,31 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="K2" t="s">
         <v>17</v>
       </c>
       <c r="L2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M2" t="s">
         <v>14</v>
@@ -569,7 +575,7 @@
         <v>16</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -580,43 +586,43 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="O3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -631,13 +637,13 @@
       <c r="E4" t="s"/>
       <c r="F4" t="s"/>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s"/>
       <c r="I4" t="s"/>
       <c r="J4" t="s"/>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="L4" t="s"/>
       <c r="M4" t="s"/>
@@ -652,25 +658,25 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
         <v>28</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
       </c>
       <c r="H5" t="s"/>
       <c r="I5" t="s"/>
       <c r="J5" t="s"/>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="L5" t="s"/>
       <c r="M5" t="s"/>
@@ -685,19 +691,23 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s"/>
-      <c r="E6" t="s"/>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
       <c r="F6" t="s"/>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s"/>
-      <c r="I6" t="s"/>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
       <c r="J6" t="s"/>
       <c r="K6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="L6" t="s"/>
       <c r="M6" t="s"/>
@@ -712,41 +722,31 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E7" t="s"/>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" t="s">
-        <v>34</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="H7" t="s"/>
       <c r="I7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="J7" t="s"/>
       <c r="K7" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" t="s">
-        <v>34</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L7" t="s"/>
       <c r="M7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" t="s">
-        <v>35</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="N7" t="s"/>
       <c r="O7" t="s"/>
     </row>
   </sheetData>

</xml_diff>